<commit_message>
added comparison with kmeans++
</commit_message>
<xml_diff>
--- a/matlab/results.xlsx
+++ b/matlab/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="42">
   <si>
     <t>alpha parameter update</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>constant alpha=diam</t>
+  </si>
+  <si>
+    <t>KMEANS++</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -798,7 +801,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -812,7 +815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -825,689 +828,747 @@
       <c r="D18">
         <v>91.429699999999997</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <f>D20/D18</f>
+        <v>0.87464576609132483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19">
+        <v>5.6890000000000001</v>
+      </c>
+      <c r="C19">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="D19">
+        <v>87.918800000000005</v>
+      </c>
+      <c r="E19">
+        <f>D20/D19</f>
+        <v>0.90957337907250768</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>62.09</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.88019999999999998</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>79.968599999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>34.619</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>0.51629999999999998</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>102.0834</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>7.0679999999999996</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>2.6800000000000001E-2</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>90.306299999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>324.24599999999998</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>4.3236999999999997</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <v>80.5197</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>62.326000000000001</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>0.86629999999999996</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>101.8554</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32">
-        <v>7.0460000000000003</v>
-      </c>
-      <c r="C32">
-        <v>2.6100000000000002E-2</v>
-      </c>
-      <c r="D32">
-        <v>92.914900000000003</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33">
-        <v>21.59</v>
+        <v>7.0460000000000003</v>
       </c>
       <c r="C33">
-        <v>0.30549999999999999</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="D33">
-        <v>79.712100000000007</v>
+        <v>92.914900000000003</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>21.59</v>
+      </c>
+      <c r="C34">
+        <v>0.30549999999999999</v>
+      </c>
+      <c r="D34">
+        <v>79.712100000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>20.893999999999998</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>0.30159999999999998</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>103.0664</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39">
-        <v>7.12</v>
-      </c>
-      <c r="C39">
-        <v>2.7699999999999999E-2</v>
-      </c>
-      <c r="D39">
-        <v>92.132000000000005</v>
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40">
-        <v>126.732</v>
+        <v>7.12</v>
       </c>
       <c r="C40">
-        <v>1.7543</v>
+        <v>2.7699999999999999E-2</v>
       </c>
       <c r="D40">
-        <v>91.297600000000003</v>
+        <v>92.132000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>126.732</v>
+      </c>
+      <c r="C41">
+        <v>1.7543</v>
+      </c>
+      <c r="D41">
+        <v>91.297600000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>48.06</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>0.69620000000000004</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>103.12130000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:4">
+      <c r="A45" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46">
-        <v>7.08</v>
-      </c>
-      <c r="C46">
-        <v>2.76E-2</v>
-      </c>
-      <c r="D46">
-        <v>90.495400000000004</v>
+        <v>16</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47">
-        <v>488.06</v>
+        <v>7.08</v>
       </c>
       <c r="C47">
-        <v>6.6741000000000001</v>
+        <v>2.76E-2</v>
       </c>
       <c r="D47">
-        <v>81.166200000000003</v>
+        <v>90.495400000000004</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>488.06</v>
+      </c>
+      <c r="C48">
+        <v>6.6741000000000001</v>
+      </c>
+      <c r="D48">
+        <v>81.166200000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>129.77000000000001</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>1.8382000000000001</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <v>102.4795</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
+    <row r="52" spans="1:5">
+      <c r="A52" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>7.9240000000000004</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>3.5451999999999997E-2</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>2427900</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1" t="s">
+      <c r="E54">
+        <f>D56/D54</f>
+        <v>0.97903538036986693</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55">
+        <v>6.74</v>
+      </c>
+      <c r="C55">
+        <v>9.3603999999999996E-3</v>
+      </c>
+      <c r="D55">
+        <v>2445800</v>
+      </c>
+      <c r="E55">
+        <f>D56/D55</f>
+        <v>0.97187014473791811</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B54">
+      <c r="B56">
         <v>70.975999999999999</v>
       </c>
-      <c r="C54">
+      <c r="C56">
         <v>1.1525000000000001</v>
       </c>
-      <c r="D54">
+      <c r="D56">
         <v>2377000</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
+    <row r="57" spans="1:5">
+      <c r="A57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B55">
+      <c r="B57">
         <v>58.037999999999997</v>
       </c>
-      <c r="C55">
+      <c r="C57">
         <v>0.96526999999999996</v>
       </c>
-      <c r="D55">
+      <c r="D57">
         <v>16674</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="3" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1" t="s">
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B60">
+      <c r="B62">
         <v>7.99</v>
       </c>
-      <c r="C60">
+      <c r="C62">
         <v>3.5674999999999998E-2</v>
       </c>
-      <c r="D60">
+      <c r="D62">
         <v>2427900</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="1" t="s">
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B61">
+      <c r="B63">
         <v>21.614000000000001</v>
       </c>
-      <c r="C61">
+      <c r="C63">
         <v>0.37558000000000002</v>
       </c>
-      <c r="D61">
+      <c r="D63">
         <v>2375400</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="1" t="s">
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B62">
+      <c r="B64">
         <v>45.78</v>
       </c>
-      <c r="C62">
+      <c r="C64">
         <v>0.77209000000000005</v>
       </c>
-      <c r="D62">
+      <c r="D64">
         <v>16630</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="3" t="s">
+    <row r="67" spans="1:4">
+      <c r="A67" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B67">
-        <v>8.01</v>
-      </c>
-      <c r="C67">
-        <v>3.6882999999999999E-2</v>
-      </c>
-      <c r="D67">
-        <v>2425700</v>
-      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68">
-        <v>53.96</v>
-      </c>
-      <c r="C68">
-        <v>0.91332999999999998</v>
-      </c>
-      <c r="D68">
-        <v>2426400</v>
+        <v>16</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69">
+        <v>8.01</v>
+      </c>
+      <c r="C69">
+        <v>3.6882999999999999E-2</v>
+      </c>
+      <c r="D69">
+        <v>2425700</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70">
+        <v>53.96</v>
+      </c>
+      <c r="C70">
+        <v>0.91332999999999998</v>
+      </c>
+      <c r="D70">
+        <v>2426400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B69">
+      <c r="B71">
         <v>50.49</v>
       </c>
-      <c r="C69">
+      <c r="C71">
         <v>0.87236999999999998</v>
       </c>
-      <c r="D69">
+      <c r="D71">
         <v>16672</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="3" t="s">
+    <row r="74" spans="1:4">
+      <c r="A74" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B74">
-        <v>3.3380000000000001</v>
-      </c>
-      <c r="C74">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="D74">
-        <v>0.39169999999999999</v>
-      </c>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B75">
-        <v>12.811</v>
-      </c>
-      <c r="C75">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="D75">
-        <v>0.29220000000000002</v>
+        <v>16</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76">
+        <v>3.3380000000000001</v>
+      </c>
+      <c r="C76">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="D76">
+        <v>0.39169999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77">
+        <v>1.4870000000000001</v>
+      </c>
+      <c r="C77">
+        <v>5.4334999999999995E-4</v>
+      </c>
+      <c r="D77">
+        <v>0.24681</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78">
+        <v>12.811</v>
+      </c>
+      <c r="C78">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D78">
+        <v>0.29220000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B76">
+      <c r="B79">
         <v>34.968000000000004</v>
       </c>
-      <c r="C76">
+      <c r="C79">
         <v>0.1421</v>
       </c>
-      <c r="D76">
+      <c r="D79">
         <v>3.0596000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="3" t="s">
+    <row r="82" spans="1:4">
+      <c r="A82" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B81">
-        <v>3.3279999999999998</v>
-      </c>
-      <c r="C81">
-        <v>4.1999999999999997E-3</v>
-      </c>
-      <c r="D81">
-        <v>0.39069999999999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B82">
-        <v>24.204000000000001</v>
-      </c>
-      <c r="C82">
-        <v>0.112</v>
-      </c>
-      <c r="D82">
-        <v>0.33389999999999997</v>
-      </c>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84">
+        <v>3.3279999999999998</v>
+      </c>
+      <c r="C84">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="D84">
+        <v>0.39069999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85">
+        <v>24.204000000000001</v>
+      </c>
+      <c r="C85">
+        <v>0.112</v>
+      </c>
+      <c r="D85">
+        <v>0.33389999999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B83">
+      <c r="B86">
         <v>32.773000000000003</v>
       </c>
-      <c r="C83">
+      <c r="C86">
         <v>0.13619999999999999</v>
       </c>
-      <c r="D83">
+      <c r="D86">
         <v>3.1701000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="3" t="s">
+    <row r="89" spans="1:4">
+      <c r="A89" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88">
-        <v>3.3090000000000002</v>
-      </c>
-      <c r="C88">
-        <v>4.1999999999999997E-3</v>
-      </c>
-      <c r="D88">
-        <v>0.39410000000000001</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B89">
-        <v>34.779000000000003</v>
-      </c>
-      <c r="C89">
-        <v>0.13420000000000001</v>
-      </c>
-      <c r="D89">
-        <v>0.32750000000000001</v>
-      </c>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91">
+        <v>3.3090000000000002</v>
+      </c>
+      <c r="C91">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="D91">
+        <v>0.39410000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92">
+        <v>34.779000000000003</v>
+      </c>
+      <c r="C92">
+        <v>0.13420000000000001</v>
+      </c>
+      <c r="D92">
+        <v>0.32750000000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B90">
+      <c r="B93">
         <v>57.668999999999997</v>
       </c>
-      <c r="C90">
+      <c r="C93">
         <v>0.2321</v>
       </c>
-      <c r="D90">
+      <c r="D93">
         <v>3.0922000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A65:D65"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A67:D67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
calc the last Psi value on both problems
</commit_message>
<xml_diff>
--- a/matlab/results.xlsx
+++ b/matlab/results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18240" windowHeight="11820"/>
@@ -156,8 +156,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,17 +222,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -278,15 +268,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="0"/>
@@ -301,7 +288,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$50</c:f>
@@ -329,7 +315,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$43</c:f>
@@ -357,7 +342,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$29</c:f>
@@ -385,7 +369,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$22</c:f>
@@ -413,7 +396,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$36</c:f>
@@ -441,7 +423,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$58</c:f>
@@ -469,7 +450,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$20</c:f>
@@ -497,7 +477,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$D$21</c:f>
@@ -511,20 +490,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="59962880"/>
-        <c:axId val="59964416"/>
+        <c:dLbls/>
+        <c:axId val="51948928"/>
+        <c:axId val="51959296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59962880"/>
+        <c:axId val="51948928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,31 +532,24 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59964416"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="51959296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59964416"/>
+        <c:axId val="51959296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59962880"/>
+        <c:crossAx val="51948928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -593,15 +557,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -609,17 +571,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -665,15 +617,12 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="0"/>
@@ -688,7 +637,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$50</c:f>
@@ -716,7 +664,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$43</c:f>
@@ -744,7 +691,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$29</c:f>
@@ -772,7 +718,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$22</c:f>
@@ -800,7 +745,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$36</c:f>
@@ -828,7 +772,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$58</c:f>
@@ -856,7 +799,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$20</c:f>
@@ -884,7 +826,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>גיליון1!$B$21</c:f>
@@ -898,20 +839,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="78722560"/>
-        <c:axId val="78724480"/>
+        <c:dLbls/>
+        <c:axId val="52365184"/>
+        <c:axId val="52379648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78722560"/>
+        <c:axId val="52365184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,32 +880,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78724480"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="52379648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78724480"/>
+        <c:axId val="52379648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78722560"/>
+        <c:crossAx val="52365184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -980,15 +906,609 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> l</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ast value comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>of Eps-KPALM with dynamic alpha updates  on Iris dataset</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>constant alpha=diam*100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>102.4795</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>constant alpha=diam*0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>103.12130000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/ln(t+2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>101.8554</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>102.0834</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/t^2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>103.0664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/2^(t-1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$D$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>103.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="77271424"/>
+        <c:axId val="77273344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="77271424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>mean</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> l</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ast</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> value</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="77273344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="77273344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77271424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean number of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> iterations </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>of </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Eps-KPALM </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>with dynamic alpha updates on Iris dataset</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>constant alpha=diam*100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>129.77000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>constant alpha=diam*0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>48.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/ln(t+2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>62.326000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>34.619</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/t^2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20.893999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>גיליון1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha0/2^(t-1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>גיליון1!$B$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>17.484000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="76463104"/>
+        <c:axId val="78686464"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="76463104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>mean</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> n</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>umber</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of iterations - log scaled</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="78686464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78686464"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76463104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1058,11 +1578,73 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1136,7 +1718,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1171,7 +1752,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1347,14 +1927,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -1364,7 +1944,7 @@
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -1374,7 +1954,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1397,7 +1977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1420,7 +2000,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1443,7 +2023,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1466,7 +2046,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1489,7 +2069,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1512,7 +2092,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1535,7 +2115,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1558,7 +2138,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1581,7 +2161,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1604,7 +2184,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1627,7 +2207,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1650,7 +2230,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1673,7 +2253,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1696,7 +2276,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1704,7 +2284,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1718,7 +2298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1732,7 +2312,7 @@
         <v>91.429699999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1746,7 +2326,7 @@
         <v>87.918800000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1760,7 +2340,7 @@
         <v>79.968599999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1774,7 +2354,7 @@
         <v>102.0834</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1782,7 +2362,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
@@ -1796,7 +2376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -1810,7 +2390,7 @@
         <v>90.306299999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
@@ -1824,7 +2404,7 @@
         <v>80.5197</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
@@ -1838,7 +2418,7 @@
         <v>101.8554</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
         <v>25</v>
       </c>
@@ -1846,7 +2426,7 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -1860,7 +2440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -1874,7 +2454,7 @@
         <v>92.914900000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1888,7 +2468,7 @@
         <v>79.712100000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1902,7 +2482,7 @@
         <v>103.0664</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
         <v>26</v>
       </c>
@@ -1910,7 +2490,7 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -1924,7 +2504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -1938,7 +2518,7 @@
         <v>92.132000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
@@ -1952,7 +2532,7 @@
         <v>91.297600000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>19</v>
       </c>
@@ -1966,7 +2546,7 @@
         <v>103.12130000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
         <v>27</v>
       </c>
@@ -1974,7 +2554,7 @@
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>16</v>
       </c>
@@ -1988,7 +2568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -2002,7 +2582,7 @@
         <v>90.495400000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>18</v>
       </c>
@@ -2016,7 +2596,7 @@
         <v>81.166200000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>19</v>
       </c>
@@ -2030,13 +2610,13 @@
         <v>102.4795</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
         <v>31</v>
       </c>
@@ -2044,7 +2624,7 @@
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
@@ -2058,7 +2638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -2072,7 +2652,7 @@
         <v>94.084000000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>40</v>
       </c>
@@ -2086,7 +2666,7 @@
         <v>89.284199999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
@@ -2100,7 +2680,7 @@
         <v>79.972999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>19</v>
       </c>
@@ -2114,7 +2694,7 @@
         <v>103.79</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="3" t="s">
         <v>32</v>
       </c>
@@ -2122,7 +2702,7 @@
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>16</v>
       </c>
@@ -2136,7 +2716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -2150,7 +2730,7 @@
         <v>2427900</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>40</v>
       </c>
@@ -2164,7 +2744,7 @@
         <v>2445800</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
         <v>18</v>
       </c>
@@ -2178,7 +2758,7 @@
         <v>2377000</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
         <v>19</v>
       </c>
@@ -2192,7 +2772,7 @@
         <v>16674</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
         <v>33</v>
       </c>
@@ -2200,7 +2780,7 @@
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
         <v>16</v>
       </c>
@@ -2214,7 +2794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -2228,7 +2808,7 @@
         <v>2427900</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
         <v>18</v>
       </c>
@@ -2242,7 +2822,7 @@
         <v>2375400</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
         <v>19</v>
       </c>
@@ -2256,7 +2836,7 @@
         <v>16630</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
         <v>35</v>
       </c>
@@ -2264,7 +2844,7 @@
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
         <v>16</v>
       </c>
@@ -2278,7 +2858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -2292,7 +2872,7 @@
         <v>2425700</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
         <v>18</v>
       </c>
@@ -2306,7 +2886,7 @@
         <v>2426400</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
         <v>19</v>
       </c>
@@ -2320,10 +2900,10 @@
         <v>16672</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="1"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="3" t="s">
         <v>44</v>
       </c>
@@ -2331,7 +2911,7 @@
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
         <v>16</v>
       </c>
@@ -2345,7 +2925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
         <v>17</v>
       </c>
@@ -2359,7 +2939,7 @@
         <v>2418100</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
         <v>40</v>
       </c>
@@ -2373,7 +2953,7 @@
         <v>2443000</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
         <v>18</v>
       </c>
@@ -2387,7 +2967,7 @@
         <v>2377000</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
         <v>19</v>
       </c>
@@ -2401,10 +2981,10 @@
         <v>15605</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="1"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="3" t="s">
         <v>36</v>
       </c>
@@ -2412,7 +2992,7 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
         <v>16</v>
       </c>
@@ -2426,7 +3006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
         <v>17</v>
       </c>
@@ -2440,7 +3020,7 @@
         <v>0.39169999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
         <v>40</v>
       </c>
@@ -2454,7 +3034,7 @@
         <v>0.24681</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
         <v>18</v>
       </c>
@@ -2468,7 +3048,7 @@
         <v>0.29220000000000002</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
         <v>19</v>
       </c>
@@ -2482,7 +3062,7 @@
         <v>3.0596000000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="3" t="s">
         <v>42</v>
       </c>
@@ -2490,7 +3070,7 @@
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="1" t="s">
         <v>16</v>
       </c>
@@ -2504,7 +3084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="1" t="s">
         <v>17</v>
       </c>
@@ -2518,7 +3098,7 @@
         <v>0.39069999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="1" t="s">
         <v>18</v>
       </c>
@@ -2532,7 +3112,7 @@
         <v>0.33389999999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="1" t="s">
         <v>19</v>
       </c>
@@ -2546,7 +3126,7 @@
         <v>3.1701000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="3" t="s">
         <v>43</v>
       </c>
@@ -2554,7 +3134,7 @@
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="1" t="s">
         <v>16</v>
       </c>
@@ -2568,7 +3148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
         <v>17</v>
       </c>
@@ -2582,7 +3162,7 @@
         <v>0.39410000000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
         <v>18</v>
       </c>
@@ -2596,7 +3176,7 @@
         <v>0.32750000000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
         <v>19</v>
       </c>
@@ -2612,6 +3192,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A40:D40"/>
     <mergeCell ref="A100:D100"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A47:D47"/>
@@ -2621,11 +3206,6 @@
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A84:D84"/>
     <mergeCell ref="A92:D92"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2634,24 +3214,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>